<commit_message>
some minor changes result display
</commit_message>
<xml_diff>
--- a/02-lab/output/excel/deformed_simplex_method_0_0.xlsx
+++ b/02-lab/output/excel/deformed_simplex_method_0_0.xlsx
@@ -53,7 +53,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -361,6 +361,105 @@
         <v>-0.0046295337444362816</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>0.3300383186754654</v>
+      </c>
+      <c r="B28" s="0">
+        <v>0.31678006652821755</v>
+      </c>
+      <c r="C28" s="0">
+        <v>-0.0046156228275238288</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0">
+        <v>0.35249483409338667</v>
+      </c>
+      <c r="B29" s="0">
+        <v>0.31824434937966328</v>
+      </c>
+      <c r="C29" s="0">
+        <v>-0.0046170387738013255</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0">
+        <v>0.32627437462854975</v>
+      </c>
+      <c r="B30" s="0">
+        <v>0.34063748112140146</v>
+      </c>
+      <c r="C30" s="0">
+        <v>-0.0046274803850593852</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0">
+        <v>0.35249483409338667</v>
+      </c>
+      <c r="B31" s="0">
+        <v>0.31824434937966328</v>
+      </c>
+      <c r="C31" s="0">
+        <v>-0.0046170387738013255</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0">
+        <v>0.33471146151821679</v>
+      </c>
+      <c r="B32" s="0">
+        <v>0.32311049088937494</v>
+      </c>
+      <c r="C32" s="0">
+        <v>-0.0046257674970918584</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0">
+        <v>0.32627437462854975</v>
+      </c>
+      <c r="B33" s="0">
+        <v>0.34063748112140146</v>
+      </c>
+      <c r="C33" s="0">
+        <v>-0.0046274803850593852</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0">
+        <v>0.33471146151821679</v>
+      </c>
+      <c r="B34" s="0">
+        <v>0.32311049088937494</v>
+      </c>
+      <c r="C34" s="0">
+        <v>-0.0046257674970918584</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>0.341493876083385</v>
+      </c>
+      <c r="B35" s="0">
+        <v>0.32505916769252574</v>
+      </c>
+      <c r="C35" s="0">
+        <v>-0.0046268147292704478</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0">
+        <v>0.32627437462854975</v>
+      </c>
+      <c r="B36" s="0">
+        <v>0.34063748112140146</v>
+      </c>
+      <c r="C36" s="0">
+        <v>-0.0046274803850593852</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>